<commit_message>
Tweaks for Norepinephrine PD modifiers.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\integration\source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CAB5E1-96B8-48BA-A012-5515C6F8B4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7260453-CF23-49A8-9D84-358CA20310B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="7035" windowWidth="27615" windowHeight="20895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4797,7 +4797,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="V16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP38" sqref="AP38"/>
+      <selection pane="bottomRight" activeCell="AX48" sqref="AX48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -15899,7 +15899,7 @@
       <c r="AN41" s="97"/>
       <c r="AO41" s="97"/>
       <c r="AP41" s="97">
-        <v>-0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="AQ41" s="97"/>
       <c r="AR41" s="97"/>
@@ -17253,7 +17253,7 @@
       <c r="AN47" s="97"/>
       <c r="AO47" s="97"/>
       <c r="AP47" s="97">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AQ47" s="97"/>
       <c r="AR47" s="97"/>

</xml_diff>

<commit_message>
Sync Data changes from rebase confusion
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\integration\source\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7260453-CF23-49A8-9D84-358CA20310B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DF66BD-B9ED-447B-A9BB-931B6907A617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="7035" windowWidth="27615" windowHeight="20895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -4793,11 +4793,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FR75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="V16" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="AH30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AX48" sqref="AX48"/>
+      <selection pane="bottomRight" activeCell="AL53" sqref="AL53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -15021,7 +15021,7 @@
       <c r="AJ37" s="97"/>
       <c r="AK37" s="97"/>
       <c r="AL37" s="97">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="AM37" s="97"/>
       <c r="AN37" s="97" t="s">
@@ -15246,13 +15246,13 @@
       <c r="AJ38" s="97"/>
       <c r="AK38" s="97"/>
       <c r="AL38" s="97">
-        <v>0.2</v>
+        <v>-0.25</v>
       </c>
       <c r="AM38" s="97"/>
       <c r="AN38" s="97"/>
       <c r="AO38" s="97"/>
       <c r="AP38" s="97">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="AQ38" s="97"/>
       <c r="AR38" s="97"/>
@@ -15893,13 +15893,13 @@
       <c r="AJ41" s="97"/>
       <c r="AK41" s="97"/>
       <c r="AL41" s="97">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="AM41" s="97"/>
       <c r="AN41" s="97"/>
       <c r="AO41" s="97"/>
       <c r="AP41" s="97">
-        <v>-0.5</v>
+        <v>-0.2</v>
       </c>
       <c r="AQ41" s="97"/>
       <c r="AR41" s="97"/>
@@ -17247,13 +17247,13 @@
       <c r="AJ47" s="97"/>
       <c r="AK47" s="97"/>
       <c r="AL47" s="97">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="AM47" s="97"/>
       <c r="AN47" s="97"/>
       <c r="AO47" s="97"/>
       <c r="AP47" s="97">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="AQ47" s="97"/>
       <c r="AR47" s="97"/>
@@ -28195,7 +28195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F226"/>
   <sheetViews>
-    <sheetView topLeftCell="A189" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
       <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
﻿Updates for norepinephrine PD. Add nervous data requests for investigating drug results.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\stress_update\source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DF66BD-B9ED-447B-A9BB-931B6907A617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C289D4B-981E-4152-8DA5-2D4126665B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28650" yWindow="9105" windowWidth="29280" windowHeight="21375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Configuration" sheetId="12" r:id="rId8"/>
     <sheet name="Tissue" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -4793,11 +4793,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FR75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AH30" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="AH21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AL53" sqref="AL53"/>
+      <selection pane="bottomRight" activeCell="AP47" sqref="AP47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -28195,7 +28195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
+    <sheetView topLeftCell="A203" workbookViewId="0">
       <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Set AdvanceToStable stabilization criteria to be the same as resting
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\stress_update\source\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C289D4B-981E-4152-8DA5-2D4126665B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55E82D-AE28-408E-9028-F3B2FFCBCE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28650" yWindow="9105" windowWidth="29280" windowHeight="21375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Configuration" sheetId="12" r:id="rId8"/>
     <sheet name="Tissue" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5331" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5318" uniqueCount="765">
   <si>
     <t>Name</t>
   </si>
@@ -2345,15 +2345,6 @@
   </si>
   <si>
     <t>AdvanceUntilStable</t>
-  </si>
-  <si>
-    <t>PartialPressure</t>
-  </si>
-  <si>
-    <t>Aorta</t>
-  </si>
-  <si>
-    <t>RespirationRate</t>
   </si>
 </sst>
 </file>
@@ -4793,7 +4784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FR75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="AH21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -28193,10 +28184,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F226"/>
+  <dimension ref="A1:F223"/>
   <sheetViews>
-    <sheetView topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="C231" sqref="C231"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="B212" sqref="B212:B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31435,7 +31426,7 @@
         <v>144</v>
       </c>
       <c r="B212" s="33">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="C212" s="30" t="s">
         <v>149</v>
@@ -31451,7 +31442,7 @@
         <v>144</v>
       </c>
       <c r="B213" s="33">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="C213" s="31" t="s">
         <v>150</v>
@@ -31467,7 +31458,7 @@
         <v>144</v>
       </c>
       <c r="B214" s="33">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="C214" s="31" t="s">
         <v>151</v>
@@ -31483,7 +31474,7 @@
         <v>144</v>
       </c>
       <c r="B215" s="33">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="C215" s="31" t="s">
         <v>152</v>
@@ -31518,7 +31509,7 @@
         <v>0.25</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>767</v>
+        <v>154</v>
       </c>
       <c r="D217" s="30" t="s">
         <v>696</v>
@@ -31531,10 +31522,10 @@
         <v>144</v>
       </c>
       <c r="B218" s="33">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>154</v>
+        <v>266</v>
       </c>
       <c r="D218" s="30" t="s">
         <v>696</v>
@@ -31550,7 +31541,7 @@
         <v>0.25</v>
       </c>
       <c r="C219" s="31" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D219" s="30" t="s">
         <v>696</v>
@@ -31559,108 +31550,52 @@
       <c r="F219" s="31"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B220" s="33">
-        <v>0.25</v>
-      </c>
-      <c r="C220" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="D220" s="30" t="s">
-        <v>696</v>
-      </c>
-      <c r="E220" s="31"/>
-      <c r="F220" s="31"/>
+      <c r="A220" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B220" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C220" s="25"/>
+      <c r="D220" s="25"/>
+      <c r="E220" s="25"/>
+      <c r="F220" s="25"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B221" s="33">
-        <v>0.25</v>
-      </c>
-      <c r="C221" s="31" t="s">
-        <v>765</v>
-      </c>
-      <c r="D221" s="31" t="s">
-        <v>692</v>
-      </c>
-      <c r="E221" s="31" t="s">
-        <v>766</v>
-      </c>
-      <c r="F221" s="31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B222" s="33">
-        <v>0.25</v>
-      </c>
-      <c r="C222" s="31" t="s">
-        <v>765</v>
-      </c>
-      <c r="D222" s="31" t="s">
-        <v>692</v>
-      </c>
-      <c r="E222" s="31" t="s">
-        <v>766</v>
-      </c>
-      <c r="F222" s="31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="B223" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="C223" s="25"/>
-      <c r="D223" s="25"/>
-      <c r="E223" s="25"/>
-      <c r="F223" s="25"/>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="24" t="s">
+      <c r="A221" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="B224" s="24" t="s">
+      <c r="B221" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C224" s="25"/>
-      <c r="D224" s="25"/>
-      <c r="E224" s="25"/>
-      <c r="F224" s="25"/>
-    </row>
-    <row r="225" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="28" t="s">
+      <c r="C221" s="25"/>
+      <c r="D221" s="25"/>
+      <c r="E221" s="25"/>
+      <c r="F221" s="25"/>
+    </row>
+    <row r="222" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B225" s="28" t="s">
+      <c r="B222" s="28" t="s">
         <v>588</v>
       </c>
-      <c r="C225" s="29"/>
-      <c r="D225" s="29"/>
-      <c r="E225" s="29"/>
-      <c r="F225" s="29"/>
-    </row>
-    <row r="226" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="32" t="s">
+      <c r="C222" s="29"/>
+      <c r="D222" s="29"/>
+      <c r="E222" s="29"/>
+      <c r="F222" s="29"/>
+    </row>
+    <row r="223" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B226" s="32" t="s">
+      <c r="B223" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C226" s="29"/>
-      <c r="D226" s="29"/>
-      <c r="E226" s="29"/>
-      <c r="F226" s="29"/>
+      <c r="C223" s="29"/>
+      <c r="D223" s="29"/>
+      <c r="E223" s="29"/>
+      <c r="F223" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added initial dehydration model.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55E82D-AE28-408E-9028-F3B2FFCBCE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B1797A-316C-4807-B05E-2D6170B70E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30735" yWindow="5430" windowWidth="25275" windowHeight="21255" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5318" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5362" uniqueCount="766">
   <si>
     <t>Name</t>
   </si>
@@ -2345,6 +2345,9 @@
   </si>
   <si>
     <t>AdvanceUntilStable</t>
+  </si>
+  <si>
+    <t>Dehydration</t>
   </si>
 </sst>
 </file>
@@ -4785,10 +4788,10 @@
   <dimension ref="A1:FR75"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AH21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AP3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP47" sqref="AP47"/>
+      <selection pane="bottomRight" activeCell="CF27" sqref="CF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -28184,10 +28187,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F223"/>
+  <dimension ref="A1:F238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="B212" sqref="B212:B219"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30035,7 +30038,7 @@
     </row>
     <row r="121" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="26" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="B121" s="27" t="s">
         <v>145</v>
@@ -30044,7 +30047,7 @@
         <v>143</v>
       </c>
       <c r="D121" s="27" t="s">
-        <v>147</v>
+        <v>695</v>
       </c>
       <c r="E121" s="27" t="s">
         <v>146</v>
@@ -30263,7 +30266,7 @@
     </row>
     <row r="136" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="26" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B136" s="27" t="s">
         <v>145</v>
@@ -30272,7 +30275,7 @@
         <v>143</v>
       </c>
       <c r="D136" s="27" t="s">
-        <v>695</v>
+        <v>147</v>
       </c>
       <c r="E136" s="27" t="s">
         <v>146</v>
@@ -30298,7 +30301,7 @@
       <c r="F137" s="30"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="30" t="s">
+      <c r="A138" s="31" t="s">
         <v>144</v>
       </c>
       <c r="B138" s="33">
@@ -30310,11 +30313,11 @@
       <c r="D138" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E138" s="30"/>
-      <c r="F138" s="30"/>
+      <c r="E138" s="31"/>
+      <c r="F138" s="31"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="30" t="s">
+      <c r="A139" s="31" t="s">
         <v>144</v>
       </c>
       <c r="B139" s="33">
@@ -30326,11 +30329,11 @@
       <c r="D139" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E139" s="30"/>
-      <c r="F139" s="30"/>
+      <c r="E139" s="31"/>
+      <c r="F139" s="31"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="30" t="s">
+      <c r="A140" s="31" t="s">
         <v>144</v>
       </c>
       <c r="B140" s="33">
@@ -30342,8 +30345,8 @@
       <c r="D140" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E140" s="30"/>
-      <c r="F140" s="30"/>
+      <c r="E140" s="31"/>
+      <c r="F140" s="31"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="31" t="s">
@@ -30491,7 +30494,7 @@
     </row>
     <row r="151" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="26" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="B151" s="27" t="s">
         <v>145</v>
@@ -30719,7 +30722,7 @@
     </row>
     <row r="166" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="26" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B166" s="27" t="s">
         <v>145</v>
@@ -30947,7 +30950,7 @@
     </row>
     <row r="181" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="26" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B181" s="27" t="s">
         <v>145</v>
@@ -31175,7 +31178,7 @@
     </row>
     <row r="196" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="26" t="s">
-        <v>689</v>
+        <v>762</v>
       </c>
       <c r="B196" s="27" t="s">
         <v>145</v>
@@ -31403,7 +31406,7 @@
     </row>
     <row r="211" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="26" t="s">
-        <v>764</v>
+        <v>689</v>
       </c>
       <c r="B211" s="27" t="s">
         <v>145</v>
@@ -31438,7 +31441,7 @@
       <c r="F212" s="30"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="31" t="s">
+      <c r="A213" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B213" s="33">
@@ -31450,11 +31453,11 @@
       <c r="D213" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E213" s="31"/>
-      <c r="F213" s="31"/>
+      <c r="E213" s="30"/>
+      <c r="F213" s="30"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="31" t="s">
+      <c r="A214" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B214" s="33">
@@ -31466,11 +31469,11 @@
       <c r="D214" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E214" s="31"/>
-      <c r="F214" s="31"/>
+      <c r="E214" s="30"/>
+      <c r="F214" s="30"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="31" t="s">
+      <c r="A215" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B215" s="33">
@@ -31482,8 +31485,8 @@
       <c r="D215" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E215" s="31"/>
-      <c r="F215" s="31"/>
+      <c r="E215" s="30"/>
+      <c r="F215" s="30"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="31" t="s">
@@ -31525,7 +31528,7 @@
         <v>0.25</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>266</v>
+        <v>586</v>
       </c>
       <c r="D218" s="30" t="s">
         <v>696</v>
@@ -31541,7 +31544,7 @@
         <v>0.25</v>
       </c>
       <c r="C219" s="31" t="s">
-        <v>267</v>
+        <v>587</v>
       </c>
       <c r="D219" s="30" t="s">
         <v>696</v>
@@ -31550,52 +31553,280 @@
       <c r="F219" s="31"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="24" t="s">
+      <c r="A220" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B220" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C220" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="D220" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E220" s="31"/>
+      <c r="F220" s="31"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B221" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C221" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="D221" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E221" s="31"/>
+      <c r="F221" s="31"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="B220" s="24" t="s">
+      <c r="B222" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="C220" s="25"/>
-      <c r="D220" s="25"/>
-      <c r="E220" s="25"/>
-      <c r="F220" s="25"/>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="24" t="s">
+      <c r="C222" s="25"/>
+      <c r="D222" s="25"/>
+      <c r="E222" s="25"/>
+      <c r="F222" s="25"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="B221" s="24" t="s">
+      <c r="B223" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C221" s="25"/>
-      <c r="D221" s="25"/>
-      <c r="E221" s="25"/>
-      <c r="F221" s="25"/>
-    </row>
-    <row r="222" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="28" t="s">
+      <c r="C223" s="25"/>
+      <c r="D223" s="25"/>
+      <c r="E223" s="25"/>
+      <c r="F223" s="25"/>
+    </row>
+    <row r="224" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B222" s="28" t="s">
+      <c r="B224" s="28" t="s">
         <v>588</v>
       </c>
-      <c r="C222" s="29"/>
-      <c r="D222" s="29"/>
-      <c r="E222" s="29"/>
-      <c r="F222" s="29"/>
-    </row>
-    <row r="223" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="32" t="s">
+      <c r="C224" s="29"/>
+      <c r="D224" s="29"/>
+      <c r="E224" s="29"/>
+      <c r="F224" s="29"/>
+    </row>
+    <row r="225" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B223" s="32" t="s">
+      <c r="B225" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C223" s="29"/>
-      <c r="D223" s="29"/>
-      <c r="E223" s="29"/>
-      <c r="F223" s="29"/>
+      <c r="C225" s="29"/>
+      <c r="D225" s="29"/>
+      <c r="E225" s="29"/>
+      <c r="F225" s="29"/>
+    </row>
+    <row r="226" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="B226" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C226" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D226" s="27" t="s">
+        <v>695</v>
+      </c>
+      <c r="E226" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F226" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="B227" s="33">
+        <v>4</v>
+      </c>
+      <c r="C227" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D227" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E227" s="30"/>
+      <c r="F227" s="30"/>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B228" s="33">
+        <v>4</v>
+      </c>
+      <c r="C228" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D228" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E228" s="31"/>
+      <c r="F228" s="31"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B229" s="33">
+        <v>4</v>
+      </c>
+      <c r="C229" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D229" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E229" s="31"/>
+      <c r="F229" s="31"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B230" s="33">
+        <v>4</v>
+      </c>
+      <c r="C230" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D230" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E230" s="31"/>
+      <c r="F230" s="31"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B231" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C231" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="D231" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E231" s="31"/>
+      <c r="F231" s="31"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B232" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C232" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="D232" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E232" s="31"/>
+      <c r="F232" s="31"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B233" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C233" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="D233" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E233" s="31"/>
+      <c r="F233" s="31"/>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B234" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C234" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="D234" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E234" s="31"/>
+      <c r="F234" s="31"/>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B235" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C235" s="25"/>
+      <c r="D235" s="25"/>
+      <c r="E235" s="25"/>
+      <c r="F235" s="25"/>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B236" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C236" s="25"/>
+      <c r="D236" s="25"/>
+      <c r="E236" s="25"/>
+      <c r="F236" s="25"/>
+    </row>
+    <row r="237" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B237" s="28" t="s">
+        <v>588</v>
+      </c>
+      <c r="C237" s="29"/>
+      <c r="D237" s="29"/>
+      <c r="E237" s="29"/>
+      <c r="F237" s="29"/>
+    </row>
+    <row r="238" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B238" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C238" s="29"/>
+      <c r="D238" s="29"/>
+      <c r="E238" s="29"/>
+      <c r="F238" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dehydration updates, including a sweat compound definition in data.xlsx.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B1797A-316C-4807-B05E-2D6170B70E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF830CF-D313-430F-8C41-DD25F4ADEDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30735" yWindow="5430" windowWidth="25275" windowHeight="21255" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="6975" windowWidth="25755" windowHeight="21330" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5362" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5405" uniqueCount="779">
   <si>
     <t>Name</t>
   </si>
@@ -2348,6 +2348,45 @@
   </si>
   <si>
     <t>Dehydration</t>
+  </si>
+  <si>
+    <t>Sweat</t>
+  </si>
+  <si>
+    <t>1.0 g/L</t>
+  </si>
+  <si>
+    <t>1.5 g/L</t>
+  </si>
+  <si>
+    <t>0.2 g/L</t>
+  </si>
+  <si>
+    <t>0.02 g/L</t>
+  </si>
+  <si>
+    <t>0.01 g/L</t>
+  </si>
+  <si>
+    <t>0.003 g/L</t>
+  </si>
+  <si>
+    <t>Sodium: 0.46-1.84 g/L (most abundant, higher levels with more intense exercise)</t>
+  </si>
+  <si>
+    <t>0.71-2.84 g/L (balances sodium concentration)</t>
+  </si>
+  <si>
+    <t>0.16-0.39 g/L (concentrations decreasing during prolonged exercise)</t>
+  </si>
+  <si>
+    <t>0-0.12 g/L (dropping significantly with increased sweat rate)</t>
+  </si>
+  <si>
+    <t>0-0.02 g/L (increases with exercise intensity and reflects muscle energy metabolism)</t>
+  </si>
+  <si>
+    <t>0.002-0.01 g/L (waste product of protein breakdown, generally higher than in blood plasma)</t>
   </si>
 </sst>
 </file>
@@ -2978,7 +3017,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3406,6 +3445,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -25954,25 +26002,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37" style="1" customWidth="1"/>
-    <col min="3" max="5" width="37" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="37" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="37" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="36.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="37" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="33" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="22.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="33" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="11" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="33" style="167" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="8.85546875" style="1" collapsed="1"/>
+    <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -26003,8 +26054,14 @@
       <c r="J1" s="60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>53</v>
       </c>
@@ -26023,8 +26080,12 @@
       <c r="J2" s="59" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="59" t="s">
+        <v>766</v>
+      </c>
+      <c r="L2" s="166"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="61" t="s">
         <v>2</v>
@@ -26053,8 +26114,14 @@
       <c r="J3" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>61</v>
       </c>
@@ -26073,8 +26140,12 @@
       <c r="J4" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" s="152"/>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>54</v>
       </c>
@@ -26093,8 +26164,14 @@
       <c r="J5" s="11" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="11" t="s">
+        <v>767</v>
+      </c>
+      <c r="L5" s="152" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="61" t="s">
         <v>2</v>
@@ -26123,8 +26200,14 @@
       <c r="J6" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
@@ -26143,8 +26226,12 @@
       <c r="J7" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K7" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="L7" s="152"/>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
@@ -26175,8 +26262,14 @@
       <c r="J8" s="11" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="11" t="s">
+        <v>768</v>
+      </c>
+      <c r="L8" s="152" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="61" t="s">
         <v>2</v>
@@ -26205,8 +26298,14 @@
       <c r="J9" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
@@ -26225,8 +26324,12 @@
       <c r="J10" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K10" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="L10" s="152"/>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -26257,8 +26360,14 @@
       <c r="J11" s="11" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="11" t="s">
+        <v>769</v>
+      </c>
+      <c r="L11" s="152" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="61" t="s">
         <v>2</v>
@@ -26287,8 +26396,14 @@
       <c r="J12" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>61</v>
       </c>
@@ -26305,8 +26420,12 @@
       <c r="J13" s="11" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="L13" s="152"/>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>54</v>
       </c>
@@ -26323,8 +26442,14 @@
       <c r="J14" s="11" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="11" t="s">
+        <v>770</v>
+      </c>
+      <c r="L14" s="152" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="61" t="s">
         <v>2</v>
@@ -26353,8 +26478,14 @@
       <c r="J15" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>61</v>
       </c>
@@ -26371,8 +26502,12 @@
       <c r="J16" s="11" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L16" s="152"/>
+    </row>
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>54</v>
       </c>
@@ -26389,8 +26524,14 @@
       <c r="J17" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="11" t="s">
+        <v>771</v>
+      </c>
+      <c r="L17" s="152" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="61" t="s">
         <v>2</v>
@@ -26419,8 +26560,14 @@
       <c r="J18" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>61</v>
       </c>
@@ -26437,8 +26584,12 @@
       <c r="J19" s="11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="L19" s="152"/>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>54</v>
       </c>
@@ -26455,8 +26606,14 @@
       <c r="J20" s="11" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="L20" s="152" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="61" t="s">
         <v>2</v>
@@ -26485,8 +26642,14 @@
       <c r="J21" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>61</v>
       </c>
@@ -26503,8 +26666,10 @@
       <c r="J22" s="11" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="11"/>
+      <c r="L22" s="152"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>54</v>
       </c>
@@ -26521,8 +26686,10 @@
       <c r="J23" s="11" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="11"/>
+      <c r="L23" s="152"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="61" t="s">
         <v>2</v>
@@ -26551,8 +26718,14 @@
       <c r="J24" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -26569,8 +26742,10 @@
       <c r="J25" s="11" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="11"/>
+      <c r="L25" s="152"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
@@ -26587,8 +26762,10 @@
       <c r="J26" s="11" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="11"/>
+      <c r="L26" s="152"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="61" t="s">
         <v>2</v>
@@ -26617,8 +26794,14 @@
       <c r="J27" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>61</v>
       </c>
@@ -26635,8 +26818,10 @@
       <c r="J28" s="11" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="11"/>
+      <c r="L28" s="152"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>54</v>
       </c>
@@ -26653,8 +26838,10 @@
       <c r="J29" s="11" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="11"/>
+      <c r="L29" s="152"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="61" t="s">
         <v>2</v>
@@ -26683,8 +26870,14 @@
       <c r="J30" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L30" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>61</v>
       </c>
@@ -26701,8 +26894,10 @@
       <c r="J31" s="11" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="11"/>
+      <c r="L31" s="152"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>54</v>
       </c>
@@ -26719,8 +26914,10 @@
       <c r="J32" s="11" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="11"/>
+      <c r="L32" s="152"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="61" t="s">
         <v>2</v>
@@ -26749,8 +26946,14 @@
       <c r="J33" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L33" s="165" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>61</v>
       </c>
@@ -26767,8 +26970,10 @@
       <c r="J34" s="11" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="11"/>
+      <c r="L34" s="152"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>54</v>
       </c>
@@ -26785,6 +26990,8 @@
       <c r="J35" s="11" t="s">
         <v>296</v>
       </c>
+      <c r="K35" s="11"/>
+      <c r="L35" s="152"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28189,8 +28396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixes for event logging.  New total fluid volume and plasma osmolality/osmolarity outputs.  General Tissue and Energy methodology improvements.  A little cleanup.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55E82D-AE28-408E-9028-F3B2FFCBCE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8448AF-BCD1-4410-A3C5-5B7A620162BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="14250" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5318" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5465" uniqueCount="780">
   <si>
     <t>Name</t>
   </si>
@@ -2345,6 +2345,51 @@
   </si>
   <si>
     <t>AdvanceUntilStable</t>
+  </si>
+  <si>
+    <t>Dehydration</t>
+  </si>
+  <si>
+    <t>Sweat</t>
+  </si>
+  <si>
+    <t>1.0 g/L</t>
+  </si>
+  <si>
+    <t>1.5 g/L</t>
+  </si>
+  <si>
+    <t>0.2 g/L</t>
+  </si>
+  <si>
+    <t>0.02 g/L</t>
+  </si>
+  <si>
+    <t>0.01 g/L</t>
+  </si>
+  <si>
+    <t>0.003 g/L</t>
+  </si>
+  <si>
+    <t>Sodium: 0.46-1.84 g/L (most abundant, higher levels with more intense exercise)</t>
+  </si>
+  <si>
+    <t>0.71-2.84 g/L (balances sodium concentration)</t>
+  </si>
+  <si>
+    <t>0.16-0.39 g/L (concentrations decreasing during prolonged exercise)</t>
+  </si>
+  <si>
+    <t>0-0.12 g/L (dropping significantly with increased sweat rate)</t>
+  </si>
+  <si>
+    <t>0-0.02 g/L (increases with exercise intensity and reflects muscle energy metabolism)</t>
+  </si>
+  <si>
+    <t>0.002-0.01 g/L (waste product of protein breakdown, generally higher than in blood plasma)</t>
+  </si>
+  <si>
+    <t>2000 s</t>
   </si>
 </sst>
 </file>
@@ -2975,7 +3020,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3367,6 +3412,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3746,34 +3800,34 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="116"/>
-      <c r="B1" s="153" t="s">
+      <c r="B1" s="156" t="s">
         <v>583</v>
       </c>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="153" t="s">
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="156" t="s">
         <v>580</v>
       </c>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="155"/>
-      <c r="J1" s="153" t="s">
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="156" t="s">
         <v>581</v>
       </c>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="154"/>
-      <c r="O1" s="154"/>
-      <c r="P1" s="154"/>
-      <c r="Q1" s="154"/>
-      <c r="R1" s="154"/>
-      <c r="S1" s="155"/>
-      <c r="T1" s="153" t="s">
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="158"/>
+      <c r="T1" s="156" t="s">
         <v>582</v>
       </c>
-      <c r="U1" s="155"/>
+      <c r="U1" s="158"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="117" t="s">
@@ -4785,10 +4839,10 @@
   <dimension ref="A1:FR75"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AH21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AP3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP47" sqref="AP47"/>
+      <selection pane="bottomRight" activeCell="CF27" sqref="CF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -25951,25 +26005,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37" style="1" customWidth="1"/>
-    <col min="3" max="5" width="37" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="37" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="37" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="36.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="37" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="33" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="22.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="33" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="22.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="33" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="22.7109375" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="33" style="155" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" collapsed="1"/>
+    <col min="19" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -26000,8 +26061,29 @@
       <c r="J1" s="60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L1" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M1" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N1" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P1" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q1" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>53</v>
       </c>
@@ -26020,8 +26102,17 @@
       <c r="J2" s="59" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59" t="s">
+        <v>766</v>
+      </c>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="154"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="61" t="s">
         <v>2</v>
@@ -26050,8 +26141,29 @@
       <c r="J3" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L3" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M3" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N3" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P3" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q3" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>61</v>
       </c>
@@ -26070,8 +26182,17 @@
       <c r="J4" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="152"/>
+    </row>
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>54</v>
       </c>
@@ -26090,8 +26211,19 @@
       <c r="J5" s="11" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11" t="s">
+        <v>767</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="152" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="61" t="s">
         <v>2</v>
@@ -26120,8 +26252,29 @@
       <c r="J6" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M6" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N6" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P6" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q6" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
@@ -26140,8 +26293,17 @@
       <c r="J7" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="152"/>
+    </row>
+    <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
@@ -26172,8 +26334,19 @@
       <c r="J8" s="11" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="152"/>
+      <c r="N8" s="11" t="s">
+        <v>768</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="152" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="61" t="s">
         <v>2</v>
@@ -26202,8 +26375,29 @@
       <c r="J9" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L9" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M9" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N9" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P9" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q9" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
@@ -26222,8 +26416,17 @@
       <c r="J10" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="152"/>
+    </row>
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -26254,8 +26457,19 @@
       <c r="J11" s="11" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="152"/>
+      <c r="N11" s="11" t="s">
+        <v>769</v>
+      </c>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="152" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="61" t="s">
         <v>2</v>
@@ -26284,8 +26498,29 @@
       <c r="J12" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L12" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M12" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N12" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P12" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q12" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>61</v>
       </c>
@@ -26302,8 +26537,17 @@
       <c r="J13" s="11" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="152"/>
+    </row>
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>54</v>
       </c>
@@ -26320,8 +26564,19 @@
       <c r="J14" s="11" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11" t="s">
+        <v>770</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="152" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="61" t="s">
         <v>2</v>
@@ -26350,8 +26605,29 @@
       <c r="J15" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L15" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M15" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N15" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P15" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q15" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>61</v>
       </c>
@@ -26368,8 +26644,17 @@
       <c r="J16" s="11" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="152"/>
+    </row>
+    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>54</v>
       </c>
@@ -26386,8 +26671,19 @@
       <c r="J17" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11" t="s">
+        <v>771</v>
+      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="152" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="61" t="s">
         <v>2</v>
@@ -26416,8 +26712,29 @@
       <c r="J18" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L18" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M18" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N18" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P18" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q18" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>61</v>
       </c>
@@ -26434,8 +26751,17 @@
       <c r="J19" s="11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="152"/>
+    </row>
+    <row r="20" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>54</v>
       </c>
@@ -26452,8 +26778,19 @@
       <c r="J20" s="11" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="152" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="61" t="s">
         <v>2</v>
@@ -26482,8 +26819,29 @@
       <c r="J21" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L21" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M21" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N21" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P21" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q21" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>61</v>
       </c>
@@ -26500,8 +26858,15 @@
       <c r="J22" s="11" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="152"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>54</v>
       </c>
@@ -26518,8 +26883,15 @@
       <c r="J23" s="11" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="152"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="61" t="s">
         <v>2</v>
@@ -26548,8 +26920,29 @@
       <c r="J24" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L24" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M24" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N24" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P24" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q24" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -26566,8 +26959,15 @@
       <c r="J25" s="11" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="152"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
@@ -26584,8 +26984,15 @@
       <c r="J26" s="11" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="152"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="61" t="s">
         <v>2</v>
@@ -26614,8 +27021,29 @@
       <c r="J27" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L27" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M27" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N27" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P27" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q27" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>61</v>
       </c>
@@ -26632,8 +27060,15 @@
       <c r="J28" s="11" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="152"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>54</v>
       </c>
@@ -26650,8 +27085,15 @@
       <c r="J29" s="11" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="152"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="61" t="s">
         <v>2</v>
@@ -26680,8 +27122,29 @@
       <c r="J30" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L30" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M30" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N30" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P30" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q30" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>61</v>
       </c>
@@ -26698,8 +27161,15 @@
       <c r="J31" s="11" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="152"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>54</v>
       </c>
@@ -26716,8 +27186,15 @@
       <c r="J32" s="11" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="152"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="61" t="s">
         <v>2</v>
@@ -26746,8 +27223,29 @@
       <c r="J33" s="61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="L33" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="M33" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="N33" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="O33" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="P33" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q33" s="153" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>61</v>
       </c>
@@ -26764,8 +27262,15 @@
       <c r="J34" s="11" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="152"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>54</v>
       </c>
@@ -26782,6 +27287,13 @@
       <c r="J35" s="11" t="s">
         <v>296</v>
       </c>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="152"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28085,19 +28597,19 @@
       <c r="B3" s="36">
         <v>3</v>
       </c>
-      <c r="C3" s="159"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
-      <c r="L3" s="160"/>
-      <c r="M3" s="160"/>
-      <c r="N3" s="160"/>
-      <c r="O3" s="161"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="163"/>
+      <c r="M3" s="163"/>
+      <c r="N3" s="163"/>
+      <c r="O3" s="164"/>
     </row>
     <row r="4" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
@@ -28106,19 +28618,19 @@
       <c r="B4" s="36" t="s">
         <v>746</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
-      <c r="K4" s="163"/>
-      <c r="L4" s="163"/>
-      <c r="M4" s="163"/>
-      <c r="N4" s="163"/>
-      <c r="O4" s="164"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
+      <c r="J4" s="166"/>
+      <c r="K4" s="166"/>
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="167"/>
     </row>
     <row r="5" spans="1:15" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="145" t="s">
@@ -28127,19 +28639,19 @@
       <c r="B5" s="146" t="s">
         <v>667</v>
       </c>
-      <c r="C5" s="156"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
-      <c r="G5" s="157"/>
-      <c r="H5" s="157"/>
-      <c r="I5" s="157"/>
-      <c r="J5" s="157"/>
-      <c r="K5" s="157"/>
-      <c r="L5" s="157"/>
-      <c r="M5" s="157"/>
-      <c r="N5" s="157"/>
-      <c r="O5" s="158"/>
+      <c r="C5" s="159"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="160"/>
+      <c r="O5" s="161"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
@@ -28184,10 +28696,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F223"/>
+  <dimension ref="A1:F238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="B212" sqref="B212:B219"/>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30035,7 +30547,7 @@
     </row>
     <row r="121" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="26" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="B121" s="27" t="s">
         <v>145</v>
@@ -30044,7 +30556,7 @@
         <v>143</v>
       </c>
       <c r="D121" s="27" t="s">
-        <v>147</v>
+        <v>695</v>
       </c>
       <c r="E121" s="27" t="s">
         <v>146</v>
@@ -30242,7 +30754,7 @@
         <v>157</v>
       </c>
       <c r="B134" s="28" t="s">
-        <v>588</v>
+        <v>779</v>
       </c>
       <c r="C134" s="29"/>
       <c r="D134" s="29"/>
@@ -30263,7 +30775,7 @@
     </row>
     <row r="136" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="26" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B136" s="27" t="s">
         <v>145</v>
@@ -30272,7 +30784,7 @@
         <v>143</v>
       </c>
       <c r="D136" s="27" t="s">
-        <v>695</v>
+        <v>147</v>
       </c>
       <c r="E136" s="27" t="s">
         <v>146</v>
@@ -30298,7 +30810,7 @@
       <c r="F137" s="30"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="30" t="s">
+      <c r="A138" s="31" t="s">
         <v>144</v>
       </c>
       <c r="B138" s="33">
@@ -30310,11 +30822,11 @@
       <c r="D138" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E138" s="30"/>
-      <c r="F138" s="30"/>
+      <c r="E138" s="31"/>
+      <c r="F138" s="31"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="30" t="s">
+      <c r="A139" s="31" t="s">
         <v>144</v>
       </c>
       <c r="B139" s="33">
@@ -30326,11 +30838,11 @@
       <c r="D139" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E139" s="30"/>
-      <c r="F139" s="30"/>
+      <c r="E139" s="31"/>
+      <c r="F139" s="31"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="30" t="s">
+      <c r="A140" s="31" t="s">
         <v>144</v>
       </c>
       <c r="B140" s="33">
@@ -30342,8 +30854,8 @@
       <c r="D140" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E140" s="30"/>
-      <c r="F140" s="30"/>
+      <c r="E140" s="31"/>
+      <c r="F140" s="31"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="31" t="s">
@@ -30491,7 +31003,7 @@
     </row>
     <row r="151" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="26" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="B151" s="27" t="s">
         <v>145</v>
@@ -30719,7 +31231,7 @@
     </row>
     <row r="166" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="26" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B166" s="27" t="s">
         <v>145</v>
@@ -30947,7 +31459,7 @@
     </row>
     <row r="181" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="26" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B181" s="27" t="s">
         <v>145</v>
@@ -31175,7 +31687,7 @@
     </row>
     <row r="196" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="26" t="s">
-        <v>689</v>
+        <v>762</v>
       </c>
       <c r="B196" s="27" t="s">
         <v>145</v>
@@ -31403,7 +31915,7 @@
     </row>
     <row r="211" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="26" t="s">
-        <v>764</v>
+        <v>689</v>
       </c>
       <c r="B211" s="27" t="s">
         <v>145</v>
@@ -31438,7 +31950,7 @@
       <c r="F212" s="30"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="31" t="s">
+      <c r="A213" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B213" s="33">
@@ -31450,11 +31962,11 @@
       <c r="D213" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E213" s="31"/>
-      <c r="F213" s="31"/>
+      <c r="E213" s="30"/>
+      <c r="F213" s="30"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="31" t="s">
+      <c r="A214" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B214" s="33">
@@ -31466,11 +31978,11 @@
       <c r="D214" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E214" s="31"/>
-      <c r="F214" s="31"/>
+      <c r="E214" s="30"/>
+      <c r="F214" s="30"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="31" t="s">
+      <c r="A215" s="30" t="s">
         <v>144</v>
       </c>
       <c r="B215" s="33">
@@ -31482,8 +31994,8 @@
       <c r="D215" s="30" t="s">
         <v>696</v>
       </c>
-      <c r="E215" s="31"/>
-      <c r="F215" s="31"/>
+      <c r="E215" s="30"/>
+      <c r="F215" s="30"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="31" t="s">
@@ -31525,7 +32037,7 @@
         <v>0.25</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>266</v>
+        <v>586</v>
       </c>
       <c r="D218" s="30" t="s">
         <v>696</v>
@@ -31541,7 +32053,7 @@
         <v>0.25</v>
       </c>
       <c r="C219" s="31" t="s">
-        <v>267</v>
+        <v>587</v>
       </c>
       <c r="D219" s="30" t="s">
         <v>696</v>
@@ -31550,52 +32062,280 @@
       <c r="F219" s="31"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="24" t="s">
+      <c r="A220" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B220" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C220" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="D220" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E220" s="31"/>
+      <c r="F220" s="31"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B221" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C221" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="D221" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E221" s="31"/>
+      <c r="F221" s="31"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="B220" s="24" t="s">
+      <c r="B222" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="C220" s="25"/>
-      <c r="D220" s="25"/>
-      <c r="E220" s="25"/>
-      <c r="F220" s="25"/>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="24" t="s">
+      <c r="C222" s="25"/>
+      <c r="D222" s="25"/>
+      <c r="E222" s="25"/>
+      <c r="F222" s="25"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="B221" s="24" t="s">
+      <c r="B223" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C221" s="25"/>
-      <c r="D221" s="25"/>
-      <c r="E221" s="25"/>
-      <c r="F221" s="25"/>
-    </row>
-    <row r="222" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="28" t="s">
+      <c r="C223" s="25"/>
+      <c r="D223" s="25"/>
+      <c r="E223" s="25"/>
+      <c r="F223" s="25"/>
+    </row>
+    <row r="224" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B222" s="28" t="s">
+      <c r="B224" s="28" t="s">
         <v>588</v>
       </c>
-      <c r="C222" s="29"/>
-      <c r="D222" s="29"/>
-      <c r="E222" s="29"/>
-      <c r="F222" s="29"/>
-    </row>
-    <row r="223" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="32" t="s">
+      <c r="C224" s="29"/>
+      <c r="D224" s="29"/>
+      <c r="E224" s="29"/>
+      <c r="F224" s="29"/>
+    </row>
+    <row r="225" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="B223" s="32" t="s">
+      <c r="B225" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C223" s="29"/>
-      <c r="D223" s="29"/>
-      <c r="E223" s="29"/>
-      <c r="F223" s="29"/>
+      <c r="C225" s="29"/>
+      <c r="D225" s="29"/>
+      <c r="E225" s="29"/>
+      <c r="F225" s="29"/>
+    </row>
+    <row r="226" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="B226" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C226" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D226" s="27" t="s">
+        <v>695</v>
+      </c>
+      <c r="E226" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F226" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="B227" s="33">
+        <v>4</v>
+      </c>
+      <c r="C227" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D227" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E227" s="30"/>
+      <c r="F227" s="30"/>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B228" s="33">
+        <v>4</v>
+      </c>
+      <c r="C228" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D228" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E228" s="31"/>
+      <c r="F228" s="31"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B229" s="33">
+        <v>4</v>
+      </c>
+      <c r="C229" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D229" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E229" s="31"/>
+      <c r="F229" s="31"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B230" s="33">
+        <v>4</v>
+      </c>
+      <c r="C230" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D230" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E230" s="31"/>
+      <c r="F230" s="31"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B231" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C231" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="D231" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E231" s="31"/>
+      <c r="F231" s="31"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B232" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C232" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="D232" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E232" s="31"/>
+      <c r="F232" s="31"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B233" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C233" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="D233" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E233" s="31"/>
+      <c r="F233" s="31"/>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B234" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="C234" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="D234" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="E234" s="31"/>
+      <c r="F234" s="31"/>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B235" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C235" s="25"/>
+      <c r="D235" s="25"/>
+      <c r="E235" s="25"/>
+      <c r="F235" s="25"/>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B236" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C236" s="25"/>
+      <c r="D236" s="25"/>
+      <c r="E236" s="25"/>
+      <c r="F236" s="25"/>
+    </row>
+    <row r="237" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B237" s="28" t="s">
+        <v>588</v>
+      </c>
+      <c r="C237" s="29"/>
+      <c r="D237" s="29"/>
+      <c r="E237" s="29"/>
+      <c r="F237" s="29"/>
+    </row>
+    <row r="238" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B238" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C238" s="29"/>
+      <c r="D238" s="29"/>
+      <c r="E238" s="29"/>
+      <c r="F238" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>